<commit_message>
fix: updated data for christmas app
</commit_message>
<xml_diff>
--- a/sheets/ice-en-xmas.xlsx
+++ b/sheets/ice-en-xmas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="List" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="curator" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="230">
   <si>
     <t>name</t>
   </si>
@@ -73,7 +73,7 @@
     <t>chu chu TV</t>
   </si>
   <si>
-    <t>"Deck The Halls"</t>
+    <t>Deck The Halls</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/KiFHi8fDKx8/mqdefault.jpg</t>
@@ -103,7 +103,7 @@
     <t>Little baby bum</t>
   </si>
   <si>
-    <t>finger family | Farmees Christmas songs</t>
+    <t>Santa Claus songs for kids | Santa Claus finger family</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/5YeXDvMqxgY/mqdefault.jpg</t>
@@ -118,7 +118,7 @@
     <t>farmees</t>
   </si>
   <si>
-    <t>Kids Christmas Songs</t>
+    <t>Where is Santa?</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/7C-FPQQOm3w/mqdefault.jpg</t>
@@ -133,7 +133,7 @@
     <t>The Kiboomers - Kids Music Channel</t>
   </si>
   <si>
-    <t>Christmas Freeze Dance</t>
+    <t>Christmas Freeze Dance | Christmas Dance Songs</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/eo9bpiwKpx4/mqdefault.jpg</t>
@@ -145,7 +145,7 @@
     <t>https://www.youtube.com/watch?v=eo9bpiwKpx4&amp;list=PL1wrsEJEvZjZmC0xYIeJxK_NYzN7mN-WD&amp;index=3</t>
   </si>
   <si>
-    <t>Christmas Tree Song</t>
+    <t>The Lights On the Christmas Tree | Christmas Tree Song</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/2ybi7qkk-T0/mqdefault.jpg</t>
@@ -157,7 +157,7 @@
     <t>https://www.youtube.com/watch?v=2ybi7qkk-T0&amp;list=PL1wrsEJEvZjZmC0xYIeJxK_NYzN7mN-WD&amp;index=10</t>
   </si>
   <si>
-    <t>We Wish You a Merry Christmas</t>
+    <t>We Wish You a Merry Christmas | Christmas Carols</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/t4-yWZrvtCM/mqdefault.jpg</t>
@@ -181,7 +181,7 @@
     <t>https://www.youtube.com/watch?v=qT6jms1yVQI&amp;list=RD6MejJBiag5A&amp;index=18</t>
   </si>
   <si>
-    <t>hristmas Carol | Christmas Songs</t>
+    <t>Jingle Bells | Christmas Carol</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/SzfvL9ioYWU/mqdefault.jpg</t>
@@ -310,9 +310,6 @@
     <t>APPUSERIES</t>
   </si>
   <si>
-    <t>kids tv christmas song</t>
-  </si>
-  <si>
     <t>https://img.youtube.com/vi/89TdgfdraUM/mqdefault.jpg</t>
   </si>
   <si>
@@ -358,7 +355,7 @@
     <t>https://www.youtube.com/watch?v=_ahmScOsvwc</t>
   </si>
   <si>
-    <t>Best Christmas Songs</t>
+    <t>Hark The Herald Angel Sings | Best Christmas Songs Of All Time</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/ntAnUWbh-Hs/mqdefault.jpg</t>
@@ -499,7 +496,7 @@
     <t>https://www.youtube.com/watch?v=0TMESkQq8lI</t>
   </si>
   <si>
-    <t>Finger Family</t>
+    <t>Finger Family Santa Claus | Nursery Rhymes</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/545Zhg65014/mqdefault.jpg</t>
@@ -535,7 +532,7 @@
     <t>https://www.youtube.com/watch?v=s2rgaLmyiFU&amp;index=4&amp;list=RDZpJCgTx_auc</t>
   </si>
   <si>
-    <t>White Christmas</t>
+    <t>White Christmas - Christmas Carol</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/DUeBeZisyjY/mqdefault.jpg</t>
@@ -661,7 +658,7 @@
     <t>The Holy Tales: Bible</t>
   </si>
   <si>
-    <t>The Christmas Tree Song</t>
+    <t>Joy To The World | The Christmas Tree Song</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/nfuTBGaEQ-E/mqdefault.jpg</t>
@@ -676,7 +673,7 @@
     <t>Kids TV 123</t>
   </si>
   <si>
-    <t>Christmas Songs</t>
+    <t>Christmas Is Coming!</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/pTFedzjmbm4/mqdefault.jpg</t>
@@ -691,7 +688,7 @@
     <t>LittleBabyBum</t>
   </si>
   <si>
-    <t>Children's Christmas Song</t>
+    <t>Hello, Reindeer | Children's Christmas Song</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/ZUi1YJVChpg/mqdefault.jpg</t>
@@ -1224,16 +1221,16 @@
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>60</v>
@@ -1241,16 +1238,16 @@
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>60</v>
@@ -1258,16 +1255,16 @@
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>60</v>
@@ -1275,16 +1272,16 @@
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>60</v>
@@ -1292,33 +1289,33 @@
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="D26" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="E26" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>123</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>34</v>
@@ -1326,84 +1323,84 @@
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="E28" s="5" t="s">
         <v>127</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>132</v>
-      </c>
       <c r="E29" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>136</v>
-      </c>
       <c r="E30" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>140</v>
-      </c>
       <c r="E31" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>98</v>
@@ -1411,16 +1408,16 @@
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="E33" s="13" t="s">
         <v>98</v>
@@ -1428,50 +1425,50 @@
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="D34" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="E34" s="13" t="s">
         <v>152</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="D35" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="E35" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="C36" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="D36" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>161</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>60</v>
@@ -1479,16 +1476,16 @@
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="D37" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>165</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>60</v>
@@ -1496,16 +1493,16 @@
     </row>
     <row r="38">
       <c r="A38" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="D38" s="4" t="s">
         <v>168</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>169</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>60</v>
@@ -1513,16 +1510,16 @@
     </row>
     <row r="39">
       <c r="A39" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="C39" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="D39" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>173</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>65</v>
@@ -1530,50 +1527,50 @@
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="C40" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="D40" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="E40" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="C41" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="D41" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="E41" s="13" t="s">
         <v>181</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="D42" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>39</v>
@@ -1581,50 +1578,50 @@
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="C43" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="D43" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="E43" s="13" t="s">
         <v>190</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="C44" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="D44" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="E44" s="9" t="s">
         <v>195</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="C45" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="D45" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>200</v>
       </c>
       <c r="E45" s="10" t="s">
         <v>39</v>
@@ -1632,104 +1629,104 @@
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="C46" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="D46" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="E46" s="9" t="s">
         <v>204</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="C47" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="D47" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="E47" s="9" t="s">
         <v>209</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="C48" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="D48" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="E48" s="9" t="s">
         <v>214</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="C49" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="D49" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="E49" s="5" t="s">
         <v>219</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="C50" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="D50" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="E50" s="13" t="s">
         <v>224</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="C51" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="D51" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="E51" s="9" t="s">
         <v>229</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="52">

</xml_diff>

<commit_message>
fix: update for christmas data
</commit_message>
<xml_diff>
--- a/sheets/ice-en-xmas.xlsx
+++ b/sheets/ice-en-xmas.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="231">
   <si>
     <t>name</t>
   </si>
@@ -103,7 +103,7 @@
     <t>Little baby bum</t>
   </si>
   <si>
-    <t>Santa Claus songs for kids | Santa Claus finger family</t>
+    <t>Santa Claus finger family for kids</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/5YeXDvMqxgY/mqdefault.jpg</t>
@@ -133,7 +133,7 @@
     <t>The Kiboomers - Kids Music Channel</t>
   </si>
   <si>
-    <t>Christmas Freeze Dance | Christmas Dance Songs</t>
+    <t>Christmas Freeze Dance songs</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/eo9bpiwKpx4/mqdefault.jpg</t>
@@ -145,7 +145,7 @@
     <t>https://www.youtube.com/watch?v=eo9bpiwKpx4&amp;list=PL1wrsEJEvZjZmC0xYIeJxK_NYzN7mN-WD&amp;index=3</t>
   </si>
   <si>
-    <t>The Lights On the Christmas Tree | Christmas Tree Song</t>
+    <t>The Lights On the Christmas Tree</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/2ybi7qkk-T0/mqdefault.jpg</t>
@@ -157,7 +157,7 @@
     <t>https://www.youtube.com/watch?v=2ybi7qkk-T0&amp;list=PL1wrsEJEvZjZmC0xYIeJxK_NYzN7mN-WD&amp;index=10</t>
   </si>
   <si>
-    <t>We Wish You a Merry Christmas | Christmas Carols</t>
+    <t>Wish You a Merry Christmas | Carols</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/t4-yWZrvtCM/mqdefault.jpg</t>
@@ -310,6 +310,9 @@
     <t>APPUSERIES</t>
   </si>
   <si>
+    <t>Christmas Carols songs</t>
+  </si>
+  <si>
     <t>https://img.youtube.com/vi/89TdgfdraUM/mqdefault.jpg</t>
   </si>
   <si>
@@ -355,7 +358,7 @@
     <t>https://www.youtube.com/watch?v=_ahmScOsvwc</t>
   </si>
   <si>
-    <t>Hark The Herald Angel Sings | Best Christmas Songs Of All Time</t>
+    <t>Hark The Herald Angel Sings</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/ntAnUWbh-Hs/mqdefault.jpg</t>
@@ -496,7 +499,7 @@
     <t>https://www.youtube.com/watch?v=0TMESkQq8lI</t>
   </si>
   <si>
-    <t>Finger Family Santa Claus | Nursery Rhymes</t>
+    <t>Finger Family Santa Claus</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/545Zhg65014/mqdefault.jpg</t>
@@ -658,7 +661,7 @@
     <t>The Holy Tales: Bible</t>
   </si>
   <si>
-    <t>Joy To The World | The Christmas Tree Song</t>
+    <t>Joy To The World song</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/nfuTBGaEQ-E/mqdefault.jpg</t>
@@ -688,7 +691,7 @@
     <t>LittleBabyBum</t>
   </si>
   <si>
-    <t>Hello, Reindeer | Children's Christmas Song</t>
+    <t>Hello, Reindeer | Children's Christmas</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/ZUi1YJVChpg/mqdefault.jpg</t>
@@ -1221,16 +1224,16 @@
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>60</v>
@@ -1238,16 +1241,16 @@
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>60</v>
@@ -1255,16 +1258,16 @@
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>60</v>
@@ -1272,16 +1275,16 @@
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>60</v>
@@ -1289,33 +1292,33 @@
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>34</v>
@@ -1323,84 +1326,84 @@
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>98</v>
@@ -1408,16 +1411,16 @@
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E33" s="13" t="s">
         <v>98</v>
@@ -1425,50 +1428,50 @@
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>60</v>
@@ -1476,16 +1479,16 @@
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>60</v>
@@ -1493,16 +1496,16 @@
     </row>
     <row r="38">
       <c r="A38" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>60</v>
@@ -1510,16 +1513,16 @@
     </row>
     <row r="39">
       <c r="A39" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>65</v>
@@ -1527,50 +1530,50 @@
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>39</v>
@@ -1578,50 +1581,50 @@
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E45" s="10" t="s">
         <v>39</v>
@@ -1629,104 +1632,104 @@
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52">

</xml_diff>